<commit_message>
removido a adição de funcionarios atualizados e utilizando realpath
</commit_message>
<xml_diff>
--- a/src/data/func_atualizado.xlsx
+++ b/src/data/func_atualizado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esocial9\Desktop\AutoJoin\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniel Costa\OneDrive\Desktop\GitHubProjetos\AutoJoin\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CADFA01-66E7-4080-9766-0A848B71D546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0886AA-D22C-41A2-AB32-D62236A068E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>RUA I</t>
+  </si>
+  <si>
+    <t>MARIA LUIZA</t>
+  </si>
+  <si>
+    <t>94585301234</t>
+  </si>
+  <si>
+    <t>RUA J</t>
+  </si>
+  <si>
+    <t>566</t>
+  </si>
+  <si>
+    <t>935859334</t>
   </si>
 </sst>
 </file>
@@ -286,8 +301,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93B1340F-00E5-44CE-B295-0FD82AEF2B06}" name="Tabela13" displayName="Tabela13" ref="A1:P9" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:P9" xr:uid="{93B1340F-00E5-44CE-B295-0FD82AEF2B06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93B1340F-00E5-44CE-B295-0FD82AEF2B06}" name="Tabela13" displayName="Tabela13" ref="A1:P10" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:P10" xr:uid="{93B1340F-00E5-44CE-B295-0FD82AEF2B06}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{9244225E-C53B-4413-8F56-641A042364AB}" name="MATRICULA" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{B7BD4B85-51F0-47F1-B55B-06C1BCDBE7FD}" name="NOME" dataDxfId="14"/>
@@ -573,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +603,7 @@
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -991,6 +1007,52 @@
         <v>931857921</v>
       </c>
       <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="1">
+        <v>52210901</v>
+      </c>
+      <c r="N10" s="1">
+        <v>83</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>